<commit_message>
implementing more multiprocessing, untested tho
</commit_message>
<xml_diff>
--- a/catalog.xlsx
+++ b/catalog.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ellio\SchoolProjects\Sumerian-Social-Network-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{968E4B81-32A5-4298-8F03-A6D4A8461A6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05270419-E8C1-4383-8921-50C17507922F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4840" yWindow="1760" windowWidth="19200" windowHeight="11170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="yearNames" sheetId="1" r:id="rId1"/>
-    <sheet name="placeNames" sheetId="2" r:id="rId2"/>
+    <sheet name="cdli_years" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1945,17 +1944,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="C111" sqref="C111"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="56.54296875" customWidth="1"/>
-    <col min="2" max="2" width="67.1796875" customWidth="1"/>
+    <col min="1" max="1" width="56.5546875" customWidth="1"/>
+    <col min="2" max="2" width="67.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1972,7 +1971,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>212</v>
       </c>
@@ -1986,7 +1985,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2000,7 +1999,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>213</v>
       </c>
@@ -2014,7 +2013,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -2028,7 +2027,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>214</v>
       </c>
@@ -2042,7 +2041,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -2056,7 +2055,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>215</v>
       </c>
@@ -2070,7 +2069,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -2084,7 +2083,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>216</v>
       </c>
@@ -2098,7 +2097,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -2112,7 +2111,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -2126,7 +2125,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -2140,7 +2139,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -2154,7 +2153,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>217</v>
       </c>
@@ -2168,7 +2167,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -2182,7 +2181,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -2196,7 +2195,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>218</v>
       </c>
@@ -2210,7 +2209,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>28</v>
       </c>
@@ -2224,7 +2223,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>220</v>
       </c>
@@ -2238,7 +2237,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -2252,7 +2251,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>32</v>
       </c>
@@ -2266,7 +2265,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -2280,7 +2279,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>36</v>
       </c>
@@ -2294,7 +2293,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>222</v>
       </c>
@@ -2308,7 +2307,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>39</v>
       </c>
@@ -2322,7 +2321,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>41</v>
       </c>
@@ -2336,7 +2335,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>43</v>
       </c>
@@ -2350,7 +2349,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>45</v>
       </c>
@@ -2364,7 +2363,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>223</v>
       </c>
@@ -2378,7 +2377,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>225</v>
       </c>
@@ -2392,7 +2391,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>47</v>
       </c>
@@ -2406,7 +2405,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>49</v>
       </c>
@@ -2420,7 +2419,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>227</v>
       </c>
@@ -2434,7 +2433,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>228</v>
       </c>
@@ -2448,7 +2447,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>229</v>
       </c>
@@ -2462,7 +2461,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>54</v>
       </c>
@@ -2476,7 +2475,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>230</v>
       </c>
@@ -2490,7 +2489,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>56</v>
       </c>
@@ -2504,7 +2503,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>58</v>
       </c>
@@ -2518,7 +2517,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>232</v>
       </c>
@@ -2532,7 +2531,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>233</v>
       </c>
@@ -2546,7 +2545,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>235</v>
       </c>
@@ -2560,7 +2559,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>87</v>
       </c>
@@ -2574,7 +2573,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>90</v>
       </c>
@@ -2588,7 +2587,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>237</v>
       </c>
@@ -2602,7 +2601,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>94</v>
       </c>
@@ -2616,7 +2615,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>97</v>
       </c>
@@ -2630,7 +2629,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>100</v>
       </c>
@@ -2644,7 +2643,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>239</v>
       </c>
@@ -2658,7 +2657,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>104</v>
       </c>
@@ -2672,7 +2671,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>107</v>
       </c>
@@ -2686,7 +2685,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>110</v>
       </c>
@@ -2703,7 +2702,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>113</v>
       </c>
@@ -2717,7 +2716,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>241</v>
       </c>
@@ -2731,7 +2730,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>242</v>
       </c>
@@ -2745,7 +2744,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>244</v>
       </c>
@@ -2759,7 +2758,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>245</v>
       </c>
@@ -2773,7 +2772,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>247</v>
       </c>
@@ -2787,7 +2786,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>249</v>
       </c>
@@ -2801,7 +2800,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>251</v>
       </c>
@@ -2815,7 +2814,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>253</v>
       </c>
@@ -2829,7 +2828,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>254</v>
       </c>
@@ -2843,7 +2842,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>256</v>
       </c>
@@ -2857,7 +2856,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>257</v>
       </c>
@@ -2871,7 +2870,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>258</v>
       </c>
@@ -2885,7 +2884,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>259</v>
       </c>
@@ -2899,7 +2898,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>260</v>
       </c>
@@ -2913,7 +2912,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>261</v>
       </c>
@@ -2927,7 +2926,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>262</v>
       </c>
@@ -2941,7 +2940,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>263</v>
       </c>
@@ -2955,7 +2954,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>265</v>
       </c>
@@ -2969,7 +2968,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>267</v>
       </c>
@@ -2983,7 +2982,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>269</v>
       </c>
@@ -2997,7 +2996,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>146</v>
       </c>
@@ -3011,7 +3010,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>271</v>
       </c>
@@ -3025,7 +3024,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>150</v>
       </c>
@@ -3039,7 +3038,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>272</v>
       </c>
@@ -3053,7 +3052,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>155</v>
       </c>
@@ -3067,7 +3066,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>273</v>
       </c>
@@ -3081,7 +3080,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>159</v>
       </c>
@@ -3095,7 +3094,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>162</v>
       </c>
@@ -3109,7 +3108,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>165</v>
       </c>
@@ -3123,7 +3122,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>275</v>
       </c>
@@ -3137,7 +3136,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>277</v>
       </c>
@@ -3151,7 +3150,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>279</v>
       </c>
@@ -3165,7 +3164,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>281</v>
       </c>
@@ -3179,7 +3178,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>283</v>
       </c>
@@ -3193,7 +3192,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>285</v>
       </c>
@@ -3207,7 +3206,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>287</v>
       </c>
@@ -3221,7 +3220,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>288</v>
       </c>
@@ -3235,7 +3234,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>289</v>
       </c>
@@ -3249,7 +3248,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>290</v>
       </c>
@@ -3263,7 +3262,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>291</v>
       </c>
@@ -3277,7 +3276,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>183</v>
       </c>
@@ -3291,7 +3290,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>185</v>
       </c>
@@ -3305,7 +3304,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>293</v>
       </c>
@@ -3319,7 +3318,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>295</v>
       </c>
@@ -3333,7 +3332,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>297</v>
       </c>
@@ -3347,7 +3346,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>299</v>
       </c>
@@ -3361,7 +3360,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>301</v>
       </c>
@@ -3375,7 +3374,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>303</v>
       </c>
@@ -3389,7 +3388,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>305</v>
       </c>
@@ -3403,7 +3402,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>307</v>
       </c>
@@ -3417,7 +3416,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>309</v>
       </c>
@@ -3431,7 +3430,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>311</v>
       </c>
@@ -3445,7 +3444,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>313</v>
       </c>
@@ -3459,7 +3458,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>315</v>
       </c>
@@ -3473,7 +3472,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>317</v>
       </c>
@@ -3487,7 +3486,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>319</v>
       </c>
@@ -3501,7 +3500,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>321</v>
       </c>
@@ -3515,7 +3514,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>323</v>
       </c>
@@ -3529,7 +3528,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>325</v>
       </c>
@@ -3543,7 +3542,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>327</v>
       </c>
@@ -3557,7 +3556,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>329</v>
       </c>
@@ -3571,7 +3570,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>331</v>
       </c>
@@ -3585,7 +3584,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>333</v>
       </c>
@@ -3599,7 +3598,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>335</v>
       </c>
@@ -3613,7 +3612,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>337</v>
       </c>
@@ -3627,7 +3626,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>339</v>
       </c>
@@ -3641,7 +3640,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>341</v>
       </c>
@@ -3655,7 +3654,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>343</v>
       </c>
@@ -3669,7 +3668,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>345</v>
       </c>
@@ -3683,7 +3682,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>347</v>
       </c>
@@ -3697,7 +3696,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>349</v>
       </c>
@@ -3711,7 +3710,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>373</v>
       </c>
@@ -3725,7 +3724,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>375</v>
       </c>
@@ -3739,7 +3738,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>377</v>
       </c>
@@ -3753,7 +3752,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>378</v>
       </c>
@@ -3767,7 +3766,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>380</v>
       </c>
@@ -3781,7 +3780,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>382</v>
       </c>
@@ -3795,7 +3794,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>384</v>
       </c>
@@ -3809,7 +3808,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>385</v>
       </c>
@@ -3823,7 +3822,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>387</v>
       </c>
@@ -3837,7 +3836,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>388</v>
       </c>
@@ -3851,7 +3850,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>391</v>
       </c>
@@ -3865,7 +3864,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>393</v>
       </c>
@@ -3879,7 +3878,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>395</v>
       </c>
@@ -3893,7 +3892,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>397</v>
       </c>
@@ -3907,7 +3906,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>399</v>
       </c>
@@ -3921,7 +3920,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>401</v>
       </c>
@@ -3935,7 +3934,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>403</v>
       </c>
@@ -3949,7 +3948,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>422</v>
       </c>
@@ -3963,7 +3962,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>424</v>
       </c>
@@ -3977,7 +3976,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>426</v>
       </c>
@@ -3991,7 +3990,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>428</v>
       </c>
@@ -4005,7 +4004,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>430</v>
       </c>
@@ -4019,7 +4018,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>432</v>
       </c>
@@ -4033,7 +4032,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>113</v>
       </c>
@@ -4047,7 +4046,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>434</v>
       </c>
@@ -4061,7 +4060,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>436</v>
       </c>
@@ -4075,7 +4074,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>438</v>
       </c>
@@ -4089,7 +4088,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>440</v>
       </c>
@@ -4103,7 +4102,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>442</v>
       </c>
@@ -4117,7 +4116,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>444</v>
       </c>
@@ -4131,7 +4130,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>446</v>
       </c>
@@ -4145,7 +4144,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>448</v>
       </c>
@@ -4159,7 +4158,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>450</v>
       </c>
@@ -4173,7 +4172,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>452</v>
       </c>
@@ -4187,7 +4186,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>454</v>
       </c>
@@ -4201,7 +4200,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>456</v>
       </c>
@@ -4215,7 +4214,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>458</v>
       </c>
@@ -4229,7 +4228,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>460</v>
       </c>
@@ -4243,7 +4242,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>462</v>
       </c>
@@ -4257,7 +4256,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>464</v>
       </c>
@@ -4271,7 +4270,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>466</v>
       </c>
@@ -4285,7 +4284,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>468</v>
       </c>
@@ -4299,7 +4298,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>470</v>
       </c>
@@ -4313,7 +4312,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>472</v>
       </c>
@@ -4327,7 +4326,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>474</v>
       </c>
@@ -4341,7 +4340,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>476</v>
       </c>
@@ -4355,7 +4354,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>478</v>
       </c>
@@ -4369,7 +4368,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>480</v>
       </c>
@@ -4383,7 +4382,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>482</v>
       </c>
@@ -4401,16 +4400,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B518ADCB-F095-4C20-AEC4-402999E93D44}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>